<commit_message>
Updating requirements and example
</commit_message>
<xml_diff>
--- a/bio2rdf-usecase/Example SciKnow.xlsx
+++ b/bio2rdf-usecase/Example SciKnow.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ana/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ana/PycharmProjects/Excel-mapping-translator/bio2rdf-usecase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7401227-E406-BD4C-ABFD-13F4229D6603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE078E8A-1678-CC44-AFDF-3048D5CBA17D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="18940" windowHeight="15500" activeTab="3" xr2:uid="{3D4B200B-6A96-B14C-B87B-4DE30C2AB37A}"/>
+    <workbookView xWindow="6660" yWindow="460" windowWidth="18940" windowHeight="15500" activeTab="1" xr2:uid="{3D4B200B-6A96-B14C-B87B-4DE30C2AB37A}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
-    <sheet name="LogicalTable" sheetId="2" r:id="rId2"/>
+    <sheet name="LogicalSource" sheetId="2" r:id="rId2"/>
     <sheet name="SubjectMap" sheetId="3" r:id="rId3"/>
     <sheet name="PredicateObjectMaps" sheetId="4" r:id="rId4"/>
     <sheet name="&lt;FunctionMap&gt;" sheetId="5" r:id="rId5"/>
@@ -233,12 +233,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -686,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E699EE22-9210-6F48-9E5D-69B648B1B634}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -774,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD44F66F-E7D2-7F41-BAFE-0A3ACFC01A10}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>